<commit_message>
Creación de la base de datos, tablas y consultas de inserción por medio de procedimientos almacenados, así como valores por defecto en algunas tablas
</commit_message>
<xml_diff>
--- a/design/Normalización Warehouse.xlsx
+++ b/design/Normalización Warehouse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\Java\JAVA\IdeaProjects\WareHouse\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0D5568-672B-41C4-8769-676ABA88B092}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C278B6D-D0FB-45E1-A9FB-1C61ABD3502C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6D862D47-D3E3-4996-9591-49F37B39E2BE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="46">
   <si>
     <t>Tablas sin normalizar</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>Salida</t>
-  </si>
-  <si>
-    <t>OrigenProducto</t>
   </si>
   <si>
     <t>Adquisicion</t>
@@ -172,7 +169,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +204,14 @@
     <font>
       <sz val="14"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -274,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -297,6 +302,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -614,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25CA8C8C-1D17-479F-9E46-457C94B6F0E4}">
-  <dimension ref="A1:Q82"/>
+  <dimension ref="A1:Q90"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="L69" sqref="L69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,30 +633,31 @@
     <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -661,7 +668,7 @@
       <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -681,22 +688,22 @@
       <c r="G4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="O4" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -704,10 +711,10 @@
       <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -730,16 +737,16 @@
       <c r="G7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="J7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="K7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="N7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="O7" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -747,7 +754,7 @@
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -767,19 +774,19 @@
       <c r="F10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="K10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="L10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N10" s="7" t="s">
+      <c r="O10" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -790,9 +797,6 @@
       <c r="E12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M12" s="2" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
@@ -822,12 +826,6 @@
       <c r="K13" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M13" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N13" s="7" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
@@ -862,21 +860,21 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>35</v>
@@ -885,32 +883,35 @@
         <v>4</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N19" s="7" t="s">
         <v>29</v>
       </c>
+      <c r="O19" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="22" spans="1:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="A22" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
+      <c r="A22" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
@@ -921,7 +922,7 @@
       <c r="F24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="J24" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -941,22 +942,22 @@
       <c r="G25" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I25" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J25" s="3" t="s">
+      <c r="J25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K25" s="3" t="s">
+      <c r="L25" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L25" s="3" t="s">
+      <c r="M25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M25" s="3" t="s">
+      <c r="N25" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N25" s="7" t="s">
+      <c r="O25" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -964,10 +965,10 @@
       <c r="B27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="K27" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M27" s="2" t="s">
+      <c r="N27" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -976,10 +977,10 @@
         <v>15</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>7</v>
@@ -993,16 +994,16 @@
       <c r="H28" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J28" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K28" s="3" t="s">
+      <c r="L28" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M28" s="5" t="s">
+      <c r="N28" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N28" s="3" t="s">
+      <c r="O28" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1010,7 +1011,7 @@
       <c r="B30" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="J30" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1030,22 +1031,22 @@
       <c r="F31" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I31" s="5" t="s">
+      <c r="J31" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J31" s="3" t="s">
+      <c r="K31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L31" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="K31" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="L31" s="3" t="s">
+      <c r="M31" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M31" s="3" t="s">
+      <c r="N31" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N31" s="7" t="s">
+      <c r="O31" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1056,9 +1057,6 @@
       <c r="E33" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M33" s="2" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
@@ -1088,18 +1086,12 @@
       <c r="K34" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M34" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N34" s="7" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M36" s="2" t="s">
+      <c r="N36" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1119,30 +1111,30 @@
       <c r="F37" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M37" s="7" t="s">
+      <c r="N37" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="N37" s="7" t="s">
+      <c r="O37" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B39" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B40" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>35</v>
@@ -1151,32 +1143,35 @@
         <v>4</v>
       </c>
       <c r="M40" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N40" s="7" t="s">
         <v>29</v>
       </c>
+      <c r="O40" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="42" spans="1:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="A42" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="8"/>
-      <c r="O42" s="8"/>
-      <c r="P42" s="8"/>
-      <c r="Q42" s="8"/>
+      <c r="A42" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="9"/>
+      <c r="O42" s="9"/>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="9"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
@@ -1187,7 +1182,7 @@
       <c r="F44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I44" s="2" t="s">
+      <c r="J44" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1207,22 +1202,22 @@
       <c r="G45" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J45" s="3" t="s">
+      <c r="J45" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K45" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K45" s="3" t="s">
+      <c r="L45" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L45" s="3" t="s">
+      <c r="M45" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M45" s="3" t="s">
+      <c r="N45" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N45" s="7" t="s">
+      <c r="O45" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1230,10 +1225,10 @@
       <c r="B47" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J47" s="2" t="s">
+      <c r="K47" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M47" s="2" t="s">
+      <c r="N47" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1242,10 +1237,10 @@
         <v>15</v>
       </c>
       <c r="C48" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>7</v>
@@ -1259,16 +1254,16 @@
       <c r="H48" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J48" s="5" t="s">
+      <c r="K48" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K48" s="3" t="s">
+      <c r="L48" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M48" s="5" t="s">
+      <c r="N48" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N48" s="3" t="s">
+      <c r="O48" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1276,7 +1271,7 @@
       <c r="B50" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I50" s="2" t="s">
+      <c r="J50" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1296,22 +1291,22 @@
       <c r="F51" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I51" s="5" t="s">
+      <c r="J51" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J51" s="3" t="s">
+      <c r="K51" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L51" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="K51" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="L51" s="3" t="s">
+      <c r="M51" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M51" s="3" t="s">
+      <c r="N51" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N51" s="7" t="s">
+      <c r="O51" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1322,9 +1317,6 @@
       <c r="E53" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M53" s="2" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B54" s="5" t="s">
@@ -1354,18 +1346,12 @@
       <c r="K54" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M54" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N54" s="7" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B56" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M56" s="2" t="s">
+      <c r="N56" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1385,30 +1371,30 @@
       <c r="F57" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M57" s="7" t="s">
+      <c r="N57" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="N57" s="7" t="s">
+      <c r="O57" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B59" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B60" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>35</v>
@@ -1417,32 +1403,35 @@
         <v>4</v>
       </c>
       <c r="M60" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N60" s="7" t="s">
         <v>29</v>
       </c>
+      <c r="O60" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="62" spans="1:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="A62" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="8"/>
-      <c r="H62" s="8"/>
-      <c r="I62" s="8"/>
-      <c r="J62" s="8"/>
-      <c r="K62" s="8"/>
-      <c r="L62" s="8"/>
-      <c r="M62" s="8"/>
-      <c r="N62" s="8"/>
-      <c r="O62" s="8"/>
-      <c r="P62" s="8"/>
-      <c r="Q62" s="8"/>
+      <c r="A62" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
+      <c r="H62" s="9"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="9"/>
+      <c r="K62" s="9"/>
+      <c r="L62" s="9"/>
+      <c r="M62" s="9"/>
+      <c r="N62" s="9"/>
+      <c r="O62" s="9"/>
+      <c r="P62" s="9"/>
+      <c r="Q62" s="9"/>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B64" s="2" t="s">
@@ -1453,11 +1442,11 @@
       <c r="F64" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I64" s="2" t="s">
+      <c r="J64" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B65" s="5" t="s">
         <v>2</v>
       </c>
@@ -1473,45 +1462,45 @@
       <c r="G65" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I65" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J65" s="3" t="s">
+      <c r="J65" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K65" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K65" s="3" t="s">
+      <c r="L65" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L65" s="3" t="s">
+      <c r="M65" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M65" s="3" t="s">
+      <c r="N65" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N65" s="7" t="s">
+      <c r="O65" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B67" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J67" s="2" t="s">
+      <c r="K67" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M67" s="2" t="s">
+      <c r="N67" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B68" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C68" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D68" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>7</v>
@@ -1525,28 +1514,28 @@
       <c r="H68" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J68" s="5" t="s">
+      <c r="K68" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K68" s="3" t="s">
+      <c r="L68" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M68" s="5" t="s">
+      <c r="N68" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N68" s="3" t="s">
+      <c r="O68" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="70" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B70" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I70" s="2" t="s">
+      <c r="J70" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B71" s="5" t="s">
         <v>2</v>
       </c>
@@ -1562,37 +1551,34 @@
       <c r="F71" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I71" s="5" t="s">
+      <c r="J71" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J71" s="3" t="s">
+      <c r="K71" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L71" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="K71" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="L71" s="3" t="s">
+      <c r="M71" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M71" s="3" t="s">
+      <c r="N71" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N71" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O71" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B73" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M73" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="74" spans="2:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B74" s="5" t="s">
         <v>26</v>
       </c>
@@ -1620,14 +1606,8 @@
       <c r="K74" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M74" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N74" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="76" spans="2:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B76" s="2" t="s">
         <v>33</v>
       </c>
@@ -1635,7 +1615,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="77" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B77" s="5" t="s">
         <v>32</v>
       </c>
@@ -1657,24 +1637,27 @@
       <c r="N77" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="79" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O77" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L79" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="80" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B80" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="M79" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="80" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B80" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>35</v>
@@ -1682,31 +1665,40 @@
       <c r="F80" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="L80" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="M80" s="7" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="N80" s="7" t="s">
-        <v>29</v>
+        <v>21</v>
+      </c>
+      <c r="O80" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="A82" s="8"/>
-      <c r="B82" s="8"/>
-      <c r="C82" s="8"/>
-      <c r="D82" s="8"/>
-      <c r="E82" s="8"/>
-      <c r="F82" s="8"/>
-      <c r="G82" s="8"/>
-      <c r="H82" s="8"/>
-      <c r="I82" s="8"/>
-      <c r="J82" s="8"/>
-      <c r="K82" s="8"/>
-      <c r="L82" s="8"/>
-      <c r="M82" s="8"/>
-      <c r="N82" s="8"/>
-      <c r="O82" s="8"/>
-      <c r="P82" s="8"/>
-      <c r="Q82" s="8"/>
+      <c r="A82" s="9"/>
+      <c r="B82" s="9"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="9"/>
+      <c r="H82" s="9"/>
+      <c r="I82" s="9"/>
+      <c r="J82" s="9"/>
+      <c r="K82" s="9"/>
+      <c r="L82" s="9"/>
+      <c r="M82" s="9"/>
+      <c r="N82" s="9"/>
+      <c r="O82" s="9"/>
+      <c r="P82" s="9"/>
+      <c r="Q82" s="9"/>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I90" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Pequeños cambios hechos a los modelos, finalización de las consultas t-sql para la aplicación
</commit_message>
<xml_diff>
--- a/design/Normalización Warehouse.xlsx
+++ b/design/Normalización Warehouse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\Java\JAVA\IdeaProjects\WareHouse\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C278B6D-D0FB-45E1-A9FB-1C61ABD3502C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A175AC-F474-4189-A748-BEBDDBFC707E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6D862D47-D3E3-4996-9591-49F37B39E2BE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="47">
   <si>
     <t>Tablas sin normalizar</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Forma Normal 3 (FN3)</t>
+  </si>
+  <si>
+    <t>OrigenProducto</t>
   </si>
 </sst>
 </file>
@@ -243,7 +246,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -275,11 +278,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -304,6 +318,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -622,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25CA8C8C-1D17-479F-9E46-457C94B6F0E4}">
   <dimension ref="A1:Q90"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="L69" sqref="L69"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12:O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -797,6 +814,9 @@
       <c r="E12" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="M12" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
@@ -824,6 +844,15 @@
         <v>26</v>
       </c>
       <c r="K13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="N13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1057,6 +1086,9 @@
       <c r="E33" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="M33" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
@@ -1084,6 +1116,15 @@
         <v>26</v>
       </c>
       <c r="K34" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M34" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="N34" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O34" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1317,6 +1358,9 @@
       <c r="E53" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="M53" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B54" s="5" t="s">
@@ -1344,6 +1388,15 @@
         <v>26</v>
       </c>
       <c r="K54" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M54" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="N54" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O54" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1577,6 +1630,9 @@
       <c r="E73" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="M73" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B74" s="5" t="s">
@@ -1604,6 +1660,15 @@
         <v>26</v>
       </c>
       <c r="K74" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M74" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="N74" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O74" s="10" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>